<commit_message>
generated the plots with the new code, adding the labels and the titles
</commit_message>
<xml_diff>
--- a/MATRICES_WORKSPACES_NEW/BLACK_SUNRISE_HSV/GLCM_All_Data_0_45_90_135_Degree/All_Data_0_45_90_135_Degree_m.xlsx
+++ b/MATRICES_WORKSPACES_NEW/BLACK_SUNRISE_HSV/GLCM_All_Data_0_45_90_135_Degree/All_Data_0_45_90_135_Degree_m.xlsx
@@ -63,2002 +63,2002 @@
   <sheetData>
     <row r="1">
       <c r="A1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
       <c r="A105">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107">
       <c r="A107">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109">
       <c r="A109">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110">
       <c r="A110">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111">
       <c r="A111">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113">
       <c r="A113">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
       <c r="A115">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117">
       <c r="A117">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118">
       <c r="A118">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119">
       <c r="A119">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120">
       <c r="A120">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121">
       <c r="A121">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122">
       <c r="A122">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124">
       <c r="A124">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127">
       <c r="A127">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128">
       <c r="A128">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129">
       <c r="A129">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130">
       <c r="A130">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131">
       <c r="A131">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132">
       <c r="A132">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133">
       <c r="A133">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134">
       <c r="A134">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135">
       <c r="A135">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136">
       <c r="A136">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137">
       <c r="A137">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138">
       <c r="A138">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139">
       <c r="A139">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140">
       <c r="A140">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141">
       <c r="A141">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142">
       <c r="A142">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
       <c r="A143">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
       <c r="A144">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145">
       <c r="A145">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
       <c r="A148">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
       <c r="A149">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
       <c r="A150">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
       <c r="A151">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
       <c r="A152">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
       <c r="A153">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
       <c r="A155">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
       <c r="A156">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157">
       <c r="A157">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
       <c r="A158">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159">
       <c r="A159">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
       <c r="A160">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161">
       <c r="A161">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162">
       <c r="A162">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163">
       <c r="A163">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="164">
       <c r="A164">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="165">
       <c r="A165">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="166">
       <c r="A166">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167">
       <c r="A167">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="168">
       <c r="A168">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169">
       <c r="A169">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170">
       <c r="A170">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171">
       <c r="A171">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="172">
       <c r="A172">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173">
       <c r="A173">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174">
       <c r="A174">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175">
       <c r="A175">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176">
       <c r="A176">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
       <c r="A177">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178">
       <c r="A178">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179">
       <c r="A179">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180">
       <c r="A180">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181">
       <c r="A181">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="182">
       <c r="A182">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183">
       <c r="A183">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="184">
       <c r="A184">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="185">
       <c r="A185">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186">
       <c r="A186">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187">
       <c r="A187">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188">
       <c r="A188">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189">
       <c r="A189">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="190">
       <c r="A190">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191">
       <c r="A191">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192">
       <c r="A192">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193">
       <c r="A193">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="194">
       <c r="A194">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195">
       <c r="A195">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="196">
       <c r="A196">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197">
       <c r="A197">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="198">
       <c r="A198">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="199">
       <c r="A199">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200">
       <c r="A200">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201">
       <c r="A201">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="202">
       <c r="A202">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="203">
       <c r="A203">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="204">
       <c r="A204">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="205">
       <c r="A205">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206">
       <c r="A206">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207">
       <c r="A207">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="208">
       <c r="A208">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="209">
       <c r="A209">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="210">
       <c r="A210">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="211">
       <c r="A211">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="212">
       <c r="A212">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213">
       <c r="A213">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
       <c r="A214">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="215">
       <c r="A215">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="216">
       <c r="A216">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="217">
       <c r="A217">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218">
       <c r="A218">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="219">
       <c r="A219">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="220">
       <c r="A220">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="221">
       <c r="A221">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="222">
       <c r="A222">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="223">
       <c r="A223">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224">
       <c r="A224">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="225">
       <c r="A225">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="226">
       <c r="A226">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="227">
       <c r="A227">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="228">
       <c r="A228">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="229">
       <c r="A229">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="230">
       <c r="A230">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="231">
       <c r="A231">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="232">
       <c r="A232">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="233">
       <c r="A233">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="234">
       <c r="A234">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="235">
       <c r="A235">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236">
       <c r="A236">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="237">
       <c r="A237">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="238">
       <c r="A238">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="239">
       <c r="A239">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="240">
       <c r="A240">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="241">
       <c r="A241">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="242">
       <c r="A242">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="243">
       <c r="A243">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244">
       <c r="A244">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245">
       <c r="A245">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="246">
       <c r="A246">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="247">
       <c r="A247">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248">
       <c r="A248">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="249">
       <c r="A249">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250">
       <c r="A250">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251">
       <c r="A251">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="252">
       <c r="A252">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="253">
       <c r="A253">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="254">
       <c r="A254">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="255">
       <c r="A255">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="256">
       <c r="A256">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257">
       <c r="A257">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="258">
       <c r="A258">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="259">
       <c r="A259">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="260">
       <c r="A260">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="261">
       <c r="A261">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="262">
       <c r="A262">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263">
       <c r="A263">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264">
       <c r="A264">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
       <c r="A265">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="266">
       <c r="A266">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="267">
       <c r="A267">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="268">
       <c r="A268">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="269">
       <c r="A269">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="270">
       <c r="A270">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="271">
       <c r="A271">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="272">
       <c r="A272">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="273">
       <c r="A273">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="274">
       <c r="A274">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="275">
       <c r="A275">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="276">
       <c r="A276">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="277">
       <c r="A277">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="278">
       <c r="A278">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279">
       <c r="A279">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="280">
       <c r="A280">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="281">
       <c r="A281">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="282">
       <c r="A282">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="283">
       <c r="A283">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="284">
       <c r="A284">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="285">
       <c r="A285">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="286">
       <c r="A286">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="287">
       <c r="A287">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="288">
       <c r="A288">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="289">
       <c r="A289">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="290">
       <c r="A290">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="291">
       <c r="A291">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="292">
       <c r="A292">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="293">
       <c r="A293">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="294">
       <c r="A294">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="295">
       <c r="A295">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="296">
       <c r="A296">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="297">
       <c r="A297">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="298">
       <c r="A298">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="299">
       <c r="A299">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="300">
       <c r="A300">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="301">
       <c r="A301">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302">
       <c r="A302">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="303">
       <c r="A303">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="304">
       <c r="A304">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305">
       <c r="A305">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="306">
       <c r="A306">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="307">
       <c r="A307">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="308">
       <c r="A308">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="309">
       <c r="A309">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="310">
       <c r="A310">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="311">
       <c r="A311">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312">
       <c r="A312">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="313">
       <c r="A313">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314">
       <c r="A314">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315">
       <c r="A315">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316">
       <c r="A316">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317">
       <c r="A317">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318">
       <c r="A318">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319">
       <c r="A319">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320">
       <c r="A320">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321">
       <c r="A321">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="322">
       <c r="A322">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="323">
       <c r="A323">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324">
       <c r="A324">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325">
       <c r="A325">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="326">
       <c r="A326">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="327">
       <c r="A327">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328">
       <c r="A328">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="329">
       <c r="A329">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="330">
       <c r="A330">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="331">
       <c r="A331">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="332">
       <c r="A332">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="333">
       <c r="A333">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="334">
       <c r="A334">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="335">
       <c r="A335">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="336">
       <c r="A336">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337">
       <c r="A337">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="338">
       <c r="A338">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="339">
       <c r="A339">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="340">
       <c r="A340">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="341">
       <c r="A341">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342">
       <c r="A342">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="343">
       <c r="A343">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="344">
       <c r="A344">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345">
       <c r="A345">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="346">
       <c r="A346">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="347">
       <c r="A347">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="348">
       <c r="A348">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="349">
       <c r="A349">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350">
       <c r="A350">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="351">
       <c r="A351">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="352">
       <c r="A352">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="353">
       <c r="A353">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="354">
       <c r="A354">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="355">
       <c r="A355">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="356">
       <c r="A356">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="357">
       <c r="A357">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="358">
       <c r="A358">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="359">
       <c r="A359">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="360">
       <c r="A360">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="361">
       <c r="A361">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="362">
       <c r="A362">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="363">
       <c r="A363">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="364">
       <c r="A364">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="365">
       <c r="A365">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="366">
       <c r="A366">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="367">
       <c r="A367">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="368">
       <c r="A368">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="369">
       <c r="A369">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="370">
       <c r="A370">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="371">
       <c r="A371">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="372">
       <c r="A372">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="373">
       <c r="A373">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="374">
       <c r="A374">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="375">
       <c r="A375">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="376">
       <c r="A376">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="377">
       <c r="A377">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="378">
       <c r="A378">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="379">
       <c r="A379">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="380">
       <c r="A380">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381">
       <c r="A381">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382">
       <c r="A382">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="383">
       <c r="A383">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="384">
       <c r="A384">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385">
       <c r="A385">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="386">
       <c r="A386">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="387">
       <c r="A387">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="388">
       <c r="A388">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389">
       <c r="A389">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="390">
       <c r="A390">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="391">
       <c r="A391">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="392">
       <c r="A392">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="393">
       <c r="A393">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394">
       <c r="A394">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="395">
       <c r="A395">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="396">
       <c r="A396">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="397">
       <c r="A397">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="398">
       <c r="A398">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="399">
       <c r="A399">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="400">
       <c r="A400">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>